<commit_message>
add excel download for queries
</commit_message>
<xml_diff>
--- a/public/uploads/target_chicago_spreadsheet.xlsx
+++ b/public/uploads/target_chicago_spreadsheet.xlsx
@@ -109,12 +109,12 @@
     <row r="1">
       <c r="A1" t="inlineStr" s="5">
         <is>
-          <t>Name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr" s="5">
         <is>
-          <t>Address</t>
+          <t>address</t>
         </is>
       </c>
     </row>
@@ -150,7 +150,7 @@
       </c>
       <c r="B4" t="inlineStr" s="5">
         <is>
-          <t>1940 W 33rd St, Chicago</t>
+          <t>1940 West 33rd Street, Chicago</t>
         </is>
       </c>
     </row>
@@ -186,7 +186,7 @@
       </c>
       <c r="B7" t="inlineStr" s="5">
         <is>
-          <t>1 S State St, Chicago</t>
+          <t>1 South State Street, Chicago</t>
         </is>
       </c>
     </row>
@@ -258,31 +258,31 @@
       </c>
       <c r="B13" t="inlineStr" s="5">
         <is>
-          <t>6525 W Diversey Ave, Chicago</t>
+          <t>6525 West Diversey Avenue, Chicago</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr" s="5">
         <is>
-          <t>Target Market News</t>
+          <t>Target</t>
         </is>
       </c>
       <c r="B14" t="inlineStr" s="5">
         <is>
-          <t>228 South Wabash Avenue, Chicago</t>
+          <t>7100 South Cicero Avenue, Bedford Park</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr" s="5">
         <is>
-          <t>Target</t>
+          <t>Target Market News</t>
         </is>
       </c>
       <c r="B15" t="inlineStr" s="5">
         <is>
-          <t>7100 South Cicero Avenue, Bedford Park</t>
+          <t>228 South Wabash Avenue, Chicago</t>
         </is>
       </c>
     </row>
@@ -294,19 +294,7 @@
       </c>
       <c r="B16" t="inlineStr" s="5">
         <is>
-          <t>6150 West Touhy Avenue, Niles</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr" s="5">
-        <is>
-          <t>Target</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr" s="5">
-        <is>
-          <t>4050 N Harlem Ave, Norridge</t>
+          <t>4050 North Harlem Avenue, Norridge</t>
         </is>
       </c>
     </row>

</xml_diff>